<commit_message>
rebase one of the demo measures
</commit_message>
<xml_diff>
--- a/inst/example_data/data.xlsx
+++ b/inst/example_data/data.xlsx
@@ -1,24 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.smith5\OneDrive - nuh.nhs.uk\Documents\R\R Package Development\ThomUK\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DD3D00-CE03-4D37-9155-306776FFA3F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week" sheetId="2" r:id="rId1"/>
     <sheet name="month" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +72,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,20 +384,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AG8" sqref="AG8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +496,7 @@
         <v>44039</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -542,52 +552,52 @@
         <v>110</v>
       </c>
       <c r="S2">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="T2">
-        <v>169</v>
+        <v>380</v>
       </c>
       <c r="U2">
-        <v>209</v>
+        <v>426</v>
       </c>
       <c r="V2">
-        <v>136</v>
+        <v>328</v>
       </c>
       <c r="W2">
-        <v>265</v>
+        <v>321</v>
       </c>
       <c r="X2">
-        <v>137</v>
+        <v>440</v>
       </c>
       <c r="Y2">
-        <v>206</v>
+        <v>310</v>
       </c>
       <c r="Z2">
-        <v>97</v>
+        <v>323</v>
       </c>
       <c r="AA2">
-        <v>68</v>
+        <v>404</v>
       </c>
       <c r="AB2">
-        <v>68</v>
+        <v>402</v>
       </c>
       <c r="AC2">
-        <v>208</v>
+        <v>422</v>
       </c>
       <c r="AD2">
-        <v>500</v>
+        <v>336</v>
       </c>
       <c r="AE2">
-        <v>321</v>
+        <v>412</v>
       </c>
       <c r="AF2">
-        <v>129</v>
+        <v>328</v>
       </c>
       <c r="AG2">
-        <v>222</v>
+        <v>385</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -688,7 +698,7 @@
         <v>0.73006131510727601</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -789,7 +799,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -890,7 +900,7 @@
         <v>0.50671363240890199</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -991,7 +1001,7 @@
         <v>0.46960140464987099</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1092,7 +1102,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1112,21 +1122,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView topLeftCell="X1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AD3" sqref="AD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1236,7 +1246,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1346,7 +1356,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1456,7 +1466,7 @@
         <v>0.35006805908237998</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1566,7 +1576,7 @@
         <v>0.56012654916340399</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1676,7 +1686,7 @@
         <v>0.38087587179121901</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1786,7 +1796,7 @@
         <v>0.396916392788075</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>0.39467874090857802</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>

</xml_diff>

<commit_message>
Update internal test data
</commit_message>
<xml_diff>
--- a/inst/example_data/data.xlsx
+++ b/inst/example_data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="none" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>ref</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>Problems</t>
-  </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>value</t>
   </si>
 </sst>
 </file>
@@ -384,19 +378,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,14 +403,20 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
+      <c r="D1" s="1">
+        <v>43890</v>
+      </c>
+      <c r="E1" s="1">
+        <v>44511</v>
+      </c>
+      <c r="F1" s="1">
+        <v>44662</v>
+      </c>
+      <c r="G1" s="1">
+        <v>44834</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>99</v>
       </c>
@@ -423,61 +426,16 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
-        <v>43890</v>
+      <c r="D2" s="2">
+        <v>60</v>
       </c>
       <c r="E2" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>99</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44511</v>
-      </c>
-      <c r="E3" s="2">
         <v>620</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>99</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44662</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="F2" s="2">
         <v>151</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1">
-        <v>44834</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="G2" s="2">
         <v>172</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add the events tab to the data sheet
</commit_message>
<xml_diff>
--- a/inst/example_data/data.xlsx
+++ b/inst/example_data/data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\francis.barton\Documents\R Projects\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD2B478-E7F2-443B-94FF-33665F4549FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="28680" yWindow="-6615" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="none" sheetId="3" r:id="rId1"/>
-    <sheet name="week" sheetId="2" r:id="rId2"/>
-    <sheet name="month" sheetId="1" r:id="rId3"/>
+    <sheet name="week" sheetId="2" r:id="rId1"/>
+    <sheet name="month" sheetId="1" r:id="rId2"/>
+    <sheet name="events" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
   <si>
     <t>ref</t>
   </si>
@@ -60,11 +61,17 @@
   <si>
     <t>Problems</t>
   </si>
+  <si>
+    <t>event_date_or_datetime</t>
+  </si>
+  <si>
+    <t>No more problems</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,10 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,88 +383,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1">
-        <v>43890</v>
-      </c>
-      <c r="E1" s="1">
-        <v>44511</v>
-      </c>
-      <c r="F1" s="1">
-        <v>44662</v>
-      </c>
-      <c r="G1" s="1">
-        <v>44834</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>99</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>60</v>
-      </c>
-      <c r="E2" s="2">
-        <v>620</v>
-      </c>
-      <c r="F2" s="2">
-        <v>151</v>
-      </c>
-      <c r="G2" s="2">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -559,7 +495,7 @@
         <v>44039</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -660,7 +596,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -761,7 +697,7 @@
         <v>0.73006131510727601</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -862,7 +798,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -963,7 +899,7 @@
         <v>0.50671363240890199</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1064,7 +1000,7 @@
         <v>0.46960140464987099</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1165,7 +1101,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1184,22 +1120,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1309,7 +1243,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1419,7 +1353,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1529,7 +1463,7 @@
         <v>0.35006805908237998</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1639,7 +1573,7 @@
         <v>0.56012654916340399</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1749,7 +1683,7 @@
         <v>0.38087587179121901</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1859,7 +1793,7 @@
         <v>0.396916392788075</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1969,7 +1903,7 @@
         <v>0.39467874090857802</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>99</v>
       </c>
@@ -2079,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2096,4 +2030,131 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1">
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
+        <v>44511</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>101</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>43890</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1">
+        <v>44511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44662</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44834</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update raw incoming example files
</commit_message>
<xml_diff>
--- a/inst/example_data/data.xlsx
+++ b/inst/example_data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD2B478-E7F2-443B-94FF-33665F4549FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B9AFB9-CF12-4BBD-8F5F-48B724404913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6615" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-6615" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week" sheetId="2" r:id="rId1"/>
@@ -1124,7 +1124,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2036,7 +2036,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2118,7 +2120,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="1">
-        <v>43890</v>
+        <v>44219</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -2129,7 +2131,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="1">
-        <v>44511</v>
+        <v>44388</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -2140,7 +2142,7 @@
         <v>12</v>
       </c>
       <c r="D8" s="1">
-        <v>44662</v>
+        <v>44562</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2151,7 +2153,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="1">
-        <v>44834</v>
+        <v>44925</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove comment col from checking functions... and example data
</commit_message>
<xml_diff>
--- a/inst/example_data/data.xlsx
+++ b/inst/example_data/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.smith5\OneDrive - nuh.nhs.uk\Documents\R\R Package Development\ThomUK\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B9AFB9-CF12-4BBD-8F5F-48B724404913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6DB4D2-1571-4A36-8743-BBE5CB408D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-6615" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="week" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
   <si>
     <t>ref</t>
   </si>
@@ -388,13 +388,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,7 +495,7 @@
         <v>44039</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -596,7 +596,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -697,7 +697,7 @@
         <v>0.73006131510727601</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -798,7 +798,7 @@
         <v>0.46</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -899,7 +899,7 @@
         <v>0.50671363240890199</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>0.46960140464987099</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1126,14 +1126,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="33" width="12" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>44805</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1353,7 +1353,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -1463,7 +1463,7 @@
         <v>0.35006805908237998</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>0.56012654916340399</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>0.38087587179121901</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>0.396916392788075</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43</v>
       </c>
@@ -1903,7 +1903,7 @@
         <v>0.39467874090857802</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>99</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -2034,21 +2034,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2056,103 +2055,94 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>99</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1">
+      <c r="C2" s="1">
         <v>43890</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>99</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="1">
         <v>44511</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>99</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="1">
         <v>44662</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>99</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="1">
         <v>44834</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>101</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1">
+      <c r="C6" s="1">
         <v>44219</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>101</v>
       </c>
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C7" s="1">
         <v>44388</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C8" s="1">
         <v>44562</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>101</v>
       </c>
       <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C9" s="1">
         <v>44925</v>
       </c>
     </row>

</xml_diff>